<commit_message>
Add agreed mark split
Agreed in Facebook Messenger chat.
</commit_message>
<xml_diff>
--- a/Final Self Assessment Form COM3504-COM6504.xlsx
+++ b/Final Self Assessment Form COM3504-COM6504.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Simon Fish</t>
   </si>
   <si>
-    <t xml:space="preserve">Scaffolded the initial app, created the Docker development environment, configured the database connection, wrote an OpenAPI schema for the JSON API, generated a stub API for developing the frontend components against, implemented a GitHub Action for linting the code with Prettier, designed and implemented all frontend components (posts, ratings bar, ratings button, navbar, base layout, user avatars and names), finalised work on Matthew’s API routes and built the rest, linked components up to API, implemented error handling, implemented caching of draft posts using IndexedDB, developed the service worker, coordinated the team using a group chat, GitHub issues for each item, and pull requests</t>
+    <t xml:space="preserve">Agreed split: 40% (1.2x base marks)</t>
   </si>
   <si>
     <t xml:space="preserve">a little bit</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Matthew Swinbank</t>
   </si>
   <si>
-    <t xml:space="preserve">Wrote the database schema using Mongoose, implemented a few API routes, and attempted to implement Socket.IO</t>
+    <t xml:space="preserve">Agreed split: 33% (1x base marks)</t>
   </si>
   <si>
     <t xml:space="preserve">fair</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Daniel Ryder</t>
   </si>
   <si>
-    <t xml:space="preserve">Attempted to implement user authentication before we knew we could use express-session</t>
+    <t xml:space="preserve">Agreed split: 27% (0.8x base marks)</t>
   </si>
   <si>
     <t xml:space="preserve">quite good</t>
@@ -156,27 +156,9 @@
     <t xml:space="preserve">it implements a web worker correctly</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">The algorithms explained in the lectures are implemented and used appropriately – genericFallback for user avatars, network-falling-back-to-cache for posts.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The only exception lies with retrieving posts. This initially would have used stale-while-revalidate, but this could not be implemented in time. Instead, network-falling-back-to-cache is used. 
+    <t xml:space="preserve">The algorithms explained in the lectures are implemented and used appropriately – genericFallback for user avatars, network-falling-back-to-cache for posts.
+The only exception lies with retrieving posts. This initially would have used stale-while-revalidate, but this could not be implemented in time. Instead, network-falling-back-to-cache is used. 
 The algorithm is selected based on the URL of the request – we use a case statement matching the URL with some regular expressions, making this quite flexible and easy for developers to change.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">It works offline</t>
@@ -374,7 +356,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -495,12 +477,6 @@
       <name val="Courier New"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -595,7 +571,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -640,7 +616,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,10 +736,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -772,11 +744,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -877,7 +849,7 @@
   <dimension ref="A1:IV88"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1187,7 @@
       <c r="E30" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="F30" s="41" t="s">
+      <c r="F30" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1258,7 +1230,7 @@
     </row>
     <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40"/>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="41" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="28" t="n">
@@ -1271,7 +1243,7 @@
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40"/>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="41" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="28" t="n">
@@ -1284,7 +1256,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40"/>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="41" t="s">
         <v>55</v>
       </c>
       <c r="E36" s="28" t="n">
@@ -1326,28 +1298,28 @@
       <c r="D39" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="43"/>
+      <c r="E39" s="42"/>
       <c r="F39" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="45"/>
+      <c r="B40" s="44"/>
       <c r="G40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="44"/>
-      <c r="B41" s="46" t="s">
+      <c r="A41" s="43"/>
+      <c r="B41" s="45" t="s">
         <v>60</v>
       </c>
       <c r="G41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="44"/>
-      <c r="B42" s="46" t="s">
+      <c r="A42" s="43"/>
+      <c r="B42" s="45" t="s">
         <v>61</v>
       </c>
       <c r="G42" s="29"/>
@@ -1386,7 +1358,7 @@
       <c r="D45" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="43"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="5" t="s">
         <v>64</v>
       </c>
@@ -1403,12 +1375,12 @@
       <c r="A48" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="45"/>
+      <c r="B48" s="44"/>
       <c r="C48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="36"/>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="41" t="s">
         <v>66</v>
       </c>
       <c r="C49" s="7"/>
@@ -1416,7 +1388,7 @@
     </row>
     <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="36"/>
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="46" t="s">
         <v>67</v>
       </c>
       <c r="C50" s="7"/>
@@ -1424,7 +1396,7 @@
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="36"/>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="41" t="s">
         <v>68</v>
       </c>
       <c r="C51" s="7"/>
@@ -1464,7 +1436,7 @@
       <c r="D54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="43"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="5" t="s">
         <v>71</v>
       </c>
@@ -1478,12 +1450,12 @@
       <c r="A56" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B56" s="45"/>
+      <c r="B56" s="44"/>
       <c r="C56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="36"/>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="41" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="7"/>
@@ -1492,7 +1464,7 @@
     </row>
     <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="36"/>
-      <c r="B58" s="47" t="s">
+      <c r="B58" s="46" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="7"/>
@@ -1529,7 +1501,7 @@
       <c r="D61" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E61" s="43"/>
+      <c r="E61" s="42"/>
       <c r="F61" s="5" t="s">
         <v>76</v>
       </c>
@@ -1549,15 +1521,15 @@
       <c r="E64" s="28"/>
     </row>
     <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="48" t="s">
+      <c r="A65" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="45"/>
+      <c r="B65" s="44"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="36"/>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="45" t="s">
         <v>78</v>
       </c>
       <c r="C66" s="7"/>
@@ -1570,7 +1542,7 @@
     </row>
     <row r="67" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="36"/>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="45" t="s">
         <v>80</v>
       </c>
       <c r="C67" s="7"/>
@@ -1609,7 +1581,7 @@
       <c r="B70" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="49"/>
+      <c r="C70" s="48"/>
       <c r="E70" s="28" t="n">
         <v>4</v>
       </c>
@@ -1623,7 +1595,7 @@
       <c r="B71" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="49"/>
+      <c r="C71" s="48"/>
       <c r="E71" s="28" t="n">
         <v>5</v>
       </c>
@@ -1714,7 +1686,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="this link"/>
+    <hyperlink ref="F13" r:id="rId1" display="Prettier was used for code formatting. All code on the master branch of our repository was formatted by Prettier. Please follow this link if you’re interested in the kinds of decisions Prettier makes as a linter.&#10;All variables use camelCase and try to be quite descriptive in what they do, except in cases relating to libraries like Express where ‘req’/’res’ are the standard for responses."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update final self-assessment form
</commit_message>
<xml_diff>
--- a/Final Self Assessment Form COM3504-COM6504.xlsx
+++ b/Final Self Assessment Form COM3504-COM6504.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
   <si>
     <t xml:space="preserve">Team Name</t>
   </si>
@@ -37,7 +37,8 @@
     <t xml:space="preserve">Simon Fish</t>
   </si>
   <si>
-    <t xml:space="preserve">Agreed split: 40% (1.2x base marks)</t>
+    <t xml:space="preserve">Agreed split: 40% (1.2x base marks)
+I completed the vast majority of the work, but I recognise that the others put in some effort to try to learn the course material. Matthew worked on the database models and Daniel was unable to contribute to the master branch.</t>
   </si>
   <si>
     <t xml:space="preserve">a little bit</t>
@@ -94,14 +95,14 @@
     <t xml:space="preserve">Code style, naming, format (consistent format regarding class and variable naming as well as indentation, consistent format regarding class and variable naming as well as indentation)</t>
   </si>
   <si>
-    <t xml:space="preserve">Prettier was used for code formatting. All code on the master branch of our repository was formatted by Prettier. Please follow this link if you’re interested in the kinds of decisions Prettier makes as a linter.
-All variables use camelCase and try to be quite descriptive in what they do, except in cases relating to libraries like Express where ‘req’/’res’ are the standard for responses.</t>
+    <t xml:space="preserve">Prettier was used for code formatting. All code on the master branch of our repository was formatted by Prettier. Please follow this link if you’re interested in the kinds of decisions Prettier makes as a linter: https://prettier.io/docs/en/rationale.html
+All variables use camelCase and try to be quite descriptive in what they do, except in cases relating to libraries like Express where ‘req’/’res’/’err’ are the standard.</t>
   </si>
   <si>
     <t xml:space="preserve">Exception (Proper use and handling of  Exceptions in your code)</t>
   </si>
   <si>
-    <t xml:space="preserve">404s are reported to the user with reason. Any other exceptions, should they arise, result in a stack trace. This would be hidden if the app was run in a production-like environment rather than a development one.</t>
+    <t xml:space="preserve">The utils.render method employed by the controller tries to ensure that appropriate response codes are sent in every situation – particularly, returning 404 in cases of looking for a nonexistent user’s wall, 400 for malformed signup input, and 500 in unprecedented cases. 500 errors result in a stack trace, which would want to be hidden if this was run in production.</t>
   </si>
   <si>
     <t xml:space="preserve">Code Organization (e.g. use of Javascript classes and modules, distribution of directories etc).  </t>
@@ -156,8 +157,7 @@
     <t xml:space="preserve">it implements a web worker correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">The algorithms explained in the lectures are implemented and used appropriately – genericFallback for user avatars, network-falling-back-to-cache for posts.
-The only exception lies with retrieving posts. This initially would have used stale-while-revalidate, but this could not be implemented in time. Instead, network-falling-back-to-cache is used. 
+    <t xml:space="preserve">The algorithms explained in the lectures are implemented and used appropriately – genericFallback for user avatars, network-falling-back-to-cache for posts, and cache-then-network for the timeline itself.
 The algorithm is selected based on the URL of the request – we use a case statement matching the URL with some regular expressions, making this quite flexible and easy for developers to change.</t>
   </si>
   <si>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">It syncs with the nodejs server</t>
   </si>
   <si>
-    <t xml:space="preserve">Unsure of what to </t>
+    <t xml:space="preserve">Not implemented</t>
   </si>
   <si>
     <t xml:space="preserve">It uses Ajax correctly</t>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t xml:space="preserve">It uses socket.io correctly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not implemented</t>
   </si>
   <si>
     <t xml:space="preserve">It syncs with the server to refresh the pages </t>
@@ -250,13 +247,13 @@
     <t xml:space="preserve">It stores images correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">Rated a 4 because we did not implement storing photos.</t>
+    <t xml:space="preserve">Rated a 3 because we did not implement storing photos.</t>
   </si>
   <si>
     <t xml:space="preserve">for example here I would focus on aspects such as efficiency and non blocking organisation</t>
   </si>
   <si>
-    <t xml:space="preserve">My implementation uses callbacks to good effect to prevent blocking threads. Failing this, async/await syntax is used on a couple of occasions.</t>
+    <t xml:space="preserve">My implementation uses callbacks to good effect to prevent blocking threads. Failing this, async/await syntax is used on a couple of occasions. It was not possible for me to implement multiple workers due to issues with authentication – res.user would come back as empty if this was used.</t>
   </si>
   <si>
     <t xml:space="preserve">4. MongoDB</t>
@@ -277,7 +274,8 @@
     <t xml:space="preserve">for example here I would expect you to let us know why you have chosen a specific organisation of the mongo modules, why the database design is appropriate (e.g. in line with my teaching) efficient and following the NoSQL organisation (i.e. you have not just created a SQL database in a different format), etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">The database was organised to roughly reflect the structure of the users/stories/ratings data we would receive, with some optimisations. Objects are linked by their IDs in the database so that they can be populated using Mongoose’s populate function during queries.</t>
+    <t xml:space="preserve">The database was organised to roughly reflect the structure of the users/stories/ratings data we would receive, with some optimisations. Objects are linked by their IDs in the database so that they can be populated using Mongoose’s populate function during queries. The files are organised as suggested in the lectures.
+Synchronisation with the local IndexedDB does not take place as I was not aware of this as a requirement, but as mentioned elsewhere, posts that fail to be submitted are saved as drafts and submitted on the next page load.</t>
   </si>
   <si>
     <t xml:space="preserve">4. Recommender algorithm</t>
@@ -325,25 +323,31 @@
     <t xml:space="preserve">Use of http and API error codes for server communication</t>
   </si>
   <si>
-    <t xml:space="preserve">The utils.render method employed by the controller tries to ensure that appropriate response codes are sent in every situation.</t>
+    <t xml:space="preserve">The utils.render method employed by the controller tries to ensure that appropriate response codes are sent in every situation – particularly, returning 404 in cases of looking for a nonexistent user’s wall, 400 for malformed signup input, and 500 in unprecedented cases.</t>
   </si>
   <si>
     <t xml:space="preserve">a login system is implemented</t>
   </si>
   <si>
-    <t xml:space="preserve">The login system is implemented, and allows the user to maintain a session. </t>
+    <t xml:space="preserve">The login system is implemented, and allows the user to maintain a session. They can sign up or log in on the first page, and the page will reload after they have done so.</t>
   </si>
   <si>
     <t xml:space="preserve">any other</t>
   </si>
   <si>
+    <t xml:space="preserve">- The route /users/me/stories was implemented to welcome the current user to their own wall.
+- Bootstrap was themed.
+- Animations were added appropriately – particularly, the rating stars have a CSS animation on click.
+- OpenAPI documentation was written to provide an overview of the application’s JSON API.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Documentation </t>
   </si>
   <si>
     <t xml:space="preserve">Code documentation: JavaDoc like /doc dir (in-line commenting, javadoc)</t>
   </si>
   <si>
-    <t xml:space="preserve">The README contains instructions on bootstrapping and seeding the app. The OpenAPI documentation documents the JSON API.</t>
+    <t xml:space="preserve">The README contains instructions on bootstrapping and seeding the app. The OpenAPI documentation at openapi.json documents the JSON API. Documentation is generated from the code using documentationjs, which can be found in doc/DOCUMENTATION.md or regenerated manually.</t>
   </si>
 </sst>
 </file>
@@ -356,7 +360,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -449,6 +453,12 @@
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -571,7 +581,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -688,19 +698,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -712,11 +726,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -736,7 +750,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,11 +758,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -756,11 +770,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -848,8 +862,8 @@
   </sheetPr>
   <dimension ref="A1:IV88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1004,7 +1018,9 @@
       <c r="A11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="28" t="n">
+        <v>5</v>
+      </c>
       <c r="F11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="153.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,11 +1045,11 @@
       <c r="E13" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="7" t="s">
         <v>25</v>
@@ -1042,7 +1058,7 @@
       <c r="E14" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="29" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1058,37 +1074,37 @@
       <c r="F15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="29"/>
+      <c r="G15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="35" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="33"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="25"/>
-      <c r="G19" s="29"/>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1101,86 +1117,86 @@
       <c r="F20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="33"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" customFormat="false" ht="1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="37"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="33"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="28"/>
-      <c r="G23" s="29"/>
+      <c r="G23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="37"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="28"/>
-      <c r="G24" s="29"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="37"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="28"/>
-      <c r="G25" s="29"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="244" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="25"/>
-      <c r="G27" s="29"/>
+      <c r="G27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="29"/>
+      <c r="G28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="41" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="25"/>
-      <c r="G29" s="29"/>
-    </row>
-    <row r="30" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="40"/>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="41"/>
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
@@ -1192,7 +1208,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="40"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="2" t="s">
         <v>45</v>
       </c>
@@ -1202,10 +1218,10 @@
       <c r="F31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="29"/>
+      <c r="G31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="40"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="2" t="s">
         <v>47</v>
       </c>
@@ -1215,10 +1231,10 @@
       <c r="F32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="29"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1226,11 +1242,11 @@
       <c r="F33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="29"/>
+      <c r="G33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41" t="s">
+      <c r="A34" s="41"/>
+      <c r="B34" s="42" t="s">
         <v>51</v>
       </c>
       <c r="E34" s="28" t="n">
@@ -1239,128 +1255,128 @@
       <c r="F34" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="29"/>
+      <c r="G34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41" t="s">
+      <c r="A35" s="41"/>
+      <c r="B35" s="42" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="28" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="41"/>
+      <c r="B36" s="42" t="s">
         <v>54</v>
-      </c>
-      <c r="G35" s="29"/>
-    </row>
-    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41" t="s">
-        <v>55</v>
       </c>
       <c r="E36" s="28" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="29"/>
+        <v>50</v>
+      </c>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="39" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="G37" s="29"/>
+      <c r="G37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E38" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="G38" s="29"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="432.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="43"/>
+      <c r="F39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="42"/>
-      <c r="F39" s="5" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="44" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="43" t="s">
+      <c r="B40" s="45"/>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="44"/>
+      <c r="B41" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="G40" s="29"/>
-    </row>
-    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="43"/>
-      <c r="B41" s="45" t="s">
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="44"/>
+      <c r="B42" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="G41" s="29"/>
-    </row>
-    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="43"/>
-      <c r="B42" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="G42" s="29"/>
+      <c r="G42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="39" t="s">
         <v>37</v>
       </c>
       <c r="E43" s="28" t="n">
         <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G43" s="29"/>
+        <v>61</v>
+      </c>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E44" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="G44" s="29"/>
+      <c r="G44" s="30"/>
     </row>
     <row r="45" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="43"/>
+      <c r="F45" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="E45" s="42"/>
-      <c r="F45" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,52 +1388,52 @@
       <c r="C47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="45"/>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="37"/>
+      <c r="B49" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="44"/>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="36"/>
-      <c r="B49" s="41" t="s">
+      <c r="C49" s="7"/>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="37"/>
+      <c r="B50" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="G49" s="29"/>
-    </row>
-    <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="36"/>
-      <c r="B50" s="46" t="s">
+      <c r="C50" s="7"/>
+      <c r="G50" s="30"/>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="37"/>
+      <c r="B51" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="G50" s="29"/>
-    </row>
-    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36"/>
-      <c r="B51" s="41" t="s">
-        <v>68</v>
-      </c>
       <c r="C51" s="7"/>
-      <c r="G51" s="29"/>
+      <c r="G51" s="30"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="39" t="s">
         <v>37</v>
       </c>
       <c r="E52" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G52" s="29"/>
+        <v>68</v>
+      </c>
+      <c r="G52" s="30"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E53" s="28" t="n">
@@ -1425,20 +1441,20 @@
       </c>
       <c r="F53" s="26"/>
     </row>
-    <row r="54" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="43"/>
+      <c r="F54" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,42 +1463,42 @@
       <c r="E55" s="28"/>
     </row>
     <row r="56" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="36" t="s">
+      <c r="A56" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="45"/>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="37"/>
+      <c r="B57" s="42" t="s">
         <v>72</v>
-      </c>
-      <c r="B56" s="44"/>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="36"/>
-      <c r="B57" s="41" t="s">
-        <v>73</v>
       </c>
       <c r="C57" s="7"/>
       <c r="F57" s="0"/>
-      <c r="G57" s="29"/>
+      <c r="G57" s="30"/>
     </row>
     <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="36"/>
-      <c r="B58" s="46" t="s">
-        <v>74</v>
+      <c r="A58" s="37"/>
+      <c r="B58" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="C58" s="7"/>
-      <c r="G58" s="29"/>
+      <c r="G58" s="30"/>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="39" t="s">
         <v>37</v>
       </c>
       <c r="E59" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="G59" s="29"/>
+      <c r="G59" s="30"/>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="39" t="s">
         <v>38</v>
       </c>
       <c r="E60" s="28" t="n">
@@ -1492,18 +1508,18 @@
     </row>
     <row r="61" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
-      <c r="B61" s="38" t="s">
+      <c r="B61" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E61" s="43"/>
+      <c r="F61" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="E61" s="42"/>
-      <c r="F61" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,109 +1537,112 @@
       <c r="E64" s="28"/>
     </row>
     <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="45"/>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="37"/>
+      <c r="B66" s="46" t="s">
         <v>77</v>
-      </c>
-      <c r="B65" s="44"/>
-      <c r="C65" s="7"/>
-    </row>
-    <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="36"/>
-      <c r="B66" s="45" t="s">
-        <v>78</v>
       </c>
       <c r="C66" s="7"/>
       <c r="E66" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F66" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="37"/>
+      <c r="B67" s="46" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="36"/>
-      <c r="B67" s="45" t="s">
-        <v>80</v>
       </c>
       <c r="C67" s="7"/>
       <c r="E67" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E68" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5"/>
       <c r="B69" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E69" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5"/>
       <c r="B70" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C70" s="48"/>
+        <v>85</v>
+      </c>
+      <c r="C70" s="49"/>
       <c r="E70" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G70" s="29"/>
-    </row>
-    <row r="71" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+      <c r="G70" s="30"/>
+    </row>
+    <row r="71" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5"/>
       <c r="B71" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C71" s="48"/>
+        <v>87</v>
+      </c>
+      <c r="C71" s="49"/>
       <c r="E71" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G71" s="29"/>
-    </row>
-    <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+      <c r="G71" s="30"/>
+    </row>
+    <row r="72" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" s="28"/>
+      <c r="F72" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E72" s="28"/>
-      <c r="G72" s="29"/>
+      <c r="G72" s="30"/>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="28"/>
-      <c r="G73" s="29"/>
+      <c r="G73" s="30"/>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="27" t="s">
         <v>91</v>
       </c>
       <c r="E74" s="28"/>
-      <c r="G74" s="29"/>
-    </row>
-    <row r="75" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="30"/>
+    </row>
+    <row r="75" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
         <v>92</v>
@@ -1642,27 +1661,27 @@
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F80" s="7"/>
-      <c r="G80" s="29"/>
+      <c r="G80" s="30"/>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="7"/>
-      <c r="G81" s="29"/>
+      <c r="G81" s="30"/>
     </row>
     <row r="82" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F82" s="7"/>
-      <c r="G82" s="29"/>
+      <c r="G82" s="30"/>
     </row>
     <row r="83" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F83" s="7"/>
-      <c r="G83" s="29"/>
+      <c r="G83" s="30"/>
     </row>
     <row r="84" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="7"/>
-      <c r="G84" s="29"/>
+      <c r="G84" s="30"/>
     </row>
     <row r="85" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F85" s="2"/>
-      <c r="G85" s="29"/>
+      <c r="G85" s="30"/>
     </row>
     <row r="86" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F86" s="26"/>
@@ -1686,7 +1705,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="Prettier was used for code formatting. All code on the master branch of our repository was formatted by Prettier. Please follow this link if you’re interested in the kinds of decisions Prettier makes as a linter.&#10;All variables use camelCase and try to be quite descriptive in what they do, except in cases relating to libraries like Express where ‘req’/’res’ are the standard for responses."/>
+    <hyperlink ref="F13" r:id="rId1" display="https://prettier.io/docs/en/rationale.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Add socketio mention to self assessment form
</commit_message>
<xml_diff>
--- a/Final Self Assessment Form COM3504-COM6504.xlsx
+++ b/Final Self Assessment Form COM3504-COM6504.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t xml:space="preserve">Team Name</t>
   </si>
@@ -177,9 +177,6 @@
     <t xml:space="preserve">It syncs with the nodejs server</t>
   </si>
   <si>
-    <t xml:space="preserve">Not implemented</t>
-  </si>
-  <si>
     <t xml:space="preserve">It uses Ajax correctly</t>
   </si>
   <si>
@@ -189,7 +186,13 @@
     <t xml:space="preserve">It uses socket.io correctly</t>
   </si>
   <si>
+    <t xml:space="preserve">When a story is created, an event is emitted. All connected clients respond to this by adding a new story to the timeline.</t>
+  </si>
+  <si>
     <t xml:space="preserve">It syncs with the server to refresh the pages </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is done through socket.io as above.</t>
   </si>
   <si>
     <r>
@@ -360,7 +363,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -453,12 +456,6 @@
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -581,7 +578,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,23 +695,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -726,11 +719,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,7 +743,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -758,11 +751,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -770,11 +763,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -862,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:IV88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1045,7 +1038,7 @@
       <c r="E13" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1058,7 +1051,7 @@
       <c r="E14" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1074,37 +1067,37 @@
       <c r="F15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="30"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="34"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="25"/>
-      <c r="G19" s="30"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1117,86 +1110,86 @@
       <c r="F20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="34"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="28"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="34"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="38"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="28"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="34"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="28"/>
-      <c r="G23" s="30"/>
+      <c r="G23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="38"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="28"/>
-      <c r="G24" s="30"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="28"/>
-      <c r="G25" s="30"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="244" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="25"/>
-      <c r="G27" s="30"/>
+      <c r="G27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="30"/>
+      <c r="G28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="25"/>
-      <c r="G29" s="30"/>
+      <c r="G29" s="29"/>
     </row>
     <row r="30" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="41"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
@@ -1208,7 +1201,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="41"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="2" t="s">
         <v>45</v>
       </c>
@@ -1218,10 +1211,10 @@
       <c r="F31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="2" t="s">
         <v>47</v>
       </c>
@@ -1231,152 +1224,149 @@
       <c r="F32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E33" s="28"/>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="40"/>
+      <c r="B34" s="41" t="s">
         <v>50</v>
-      </c>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41"/>
-      <c r="B34" s="42" t="s">
-        <v>51</v>
       </c>
       <c r="E34" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="29"/>
+    </row>
+    <row r="35" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="40"/>
+      <c r="B35" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="30"/>
-    </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41"/>
-      <c r="B35" s="42" t="s">
+      <c r="E35" s="28" t="n">
+        <v>5</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41"/>
-      <c r="B36" s="42" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="41" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="28" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="G36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="38" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="38" t="s">
         <v>38</v>
       </c>
       <c r="E38" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="G38" s="30"/>
+      <c r="G38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="432.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="43"/>
+        <v>57</v>
+      </c>
+      <c r="E39" s="42"/>
       <c r="F39" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="45"/>
-      <c r="G40" s="30"/>
+      <c r="A40" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="44"/>
+      <c r="G40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="44"/>
-      <c r="B41" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" s="30"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="44"/>
-      <c r="B42" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="G42" s="30"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="38" t="s">
         <v>37</v>
       </c>
       <c r="E43" s="28" t="n">
         <v>3</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G43" s="30"/>
+        <v>62</v>
+      </c>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="38" t="s">
         <v>38</v>
       </c>
       <c r="E44" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="G44" s="30"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E45" s="43"/>
+        <v>63</v>
+      </c>
+      <c r="E45" s="42"/>
       <c r="F45" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,52 +1378,52 @@
       <c r="C47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="45"/>
+      <c r="A48" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="44"/>
       <c r="C48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="37"/>
-      <c r="B49" s="42" t="s">
-        <v>65</v>
+      <c r="A49" s="36"/>
+      <c r="B49" s="41" t="s">
+        <v>66</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="G49" s="30"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="37"/>
-      <c r="B50" s="47" t="s">
-        <v>66</v>
+      <c r="A50" s="36"/>
+      <c r="B50" s="46" t="s">
+        <v>67</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="G50" s="30"/>
+      <c r="G50" s="29"/>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="37"/>
-      <c r="B51" s="42" t="s">
-        <v>67</v>
+      <c r="A51" s="36"/>
+      <c r="B51" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="G51" s="30"/>
+      <c r="G51" s="29"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="38" t="s">
         <v>37</v>
       </c>
       <c r="E52" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="30"/>
+        <v>69</v>
+      </c>
+      <c r="G52" s="29"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="38" t="s">
         <v>38</v>
       </c>
       <c r="E53" s="28" t="n">
@@ -1443,18 +1433,18 @@
     </row>
     <row r="54" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
-      <c r="B54" s="39" t="s">
+      <c r="B54" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" s="43"/>
+        <v>70</v>
+      </c>
+      <c r="E54" s="42"/>
       <c r="F54" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,42 +1453,42 @@
       <c r="E55" s="28"/>
     </row>
     <row r="56" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="45"/>
+      <c r="A56" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="44"/>
       <c r="C56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="37"/>
-      <c r="B57" s="42" t="s">
-        <v>72</v>
+      <c r="A57" s="36"/>
+      <c r="B57" s="41" t="s">
+        <v>73</v>
       </c>
       <c r="C57" s="7"/>
       <c r="F57" s="0"/>
-      <c r="G57" s="30"/>
+      <c r="G57" s="29"/>
     </row>
     <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="37"/>
-      <c r="B58" s="47" t="s">
-        <v>73</v>
+      <c r="A58" s="36"/>
+      <c r="B58" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="C58" s="7"/>
-      <c r="G58" s="30"/>
+      <c r="G58" s="29"/>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="38" t="s">
         <v>37</v>
       </c>
       <c r="E59" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="G59" s="30"/>
+      <c r="G59" s="29"/>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
-      <c r="B60" s="39" t="s">
+      <c r="B60" s="38" t="s">
         <v>38</v>
       </c>
       <c r="E60" s="28" t="n">
@@ -1508,18 +1498,18 @@
     </row>
     <row r="61" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E61" s="43"/>
+        <v>75</v>
+      </c>
+      <c r="E61" s="42"/>
       <c r="F61" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,120 +1527,120 @@
       <c r="E64" s="28"/>
     </row>
     <row r="65" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="45"/>
+      <c r="A65" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="44"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="37"/>
-      <c r="B66" s="46" t="s">
-        <v>77</v>
+      <c r="A66" s="36"/>
+      <c r="B66" s="45" t="s">
+        <v>78</v>
       </c>
       <c r="C66" s="7"/>
       <c r="E66" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="37"/>
-      <c r="B67" s="46" t="s">
-        <v>79</v>
+      <c r="A67" s="36"/>
+      <c r="B67" s="45" t="s">
+        <v>80</v>
       </c>
       <c r="C67" s="7"/>
       <c r="E67" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E68" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5"/>
       <c r="B69" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E69" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5"/>
       <c r="B70" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C70" s="49"/>
+        <v>86</v>
+      </c>
+      <c r="C70" s="48"/>
       <c r="E70" s="28" t="n">
         <v>4</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G70" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="G70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5"/>
       <c r="B71" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C71" s="49"/>
+        <v>88</v>
+      </c>
+      <c r="C71" s="48"/>
       <c r="E71" s="28" t="n">
         <v>5</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G71" s="30"/>
+        <v>89</v>
+      </c>
+      <c r="G71" s="29"/>
     </row>
     <row r="72" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5"/>
       <c r="B72" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E72" s="28"/>
       <c r="F72" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G72" s="30"/>
+        <v>91</v>
+      </c>
+      <c r="G72" s="29"/>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="28"/>
-      <c r="G73" s="30"/>
+      <c r="G73" s="29"/>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E74" s="28"/>
-      <c r="G74" s="30"/>
+      <c r="G74" s="29"/>
     </row>
     <row r="75" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5"/>
       <c r="B75" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C75" s="7"/>
       <c r="E75" s="28"/>
       <c r="F75" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,27 +1651,27 @@
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F80" s="7"/>
-      <c r="G80" s="30"/>
+      <c r="G80" s="29"/>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F81" s="7"/>
-      <c r="G81" s="30"/>
+      <c r="G81" s="29"/>
     </row>
     <row r="82" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F82" s="7"/>
-      <c r="G82" s="30"/>
+      <c r="G82" s="29"/>
     </row>
     <row r="83" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F83" s="7"/>
-      <c r="G83" s="30"/>
+      <c r="G83" s="29"/>
     </row>
     <row r="84" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F84" s="7"/>
-      <c r="G84" s="30"/>
+      <c r="G84" s="29"/>
     </row>
     <row r="85" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F85" s="2"/>
-      <c r="G85" s="30"/>
+      <c r="G85" s="29"/>
     </row>
     <row r="86" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F86" s="26"/>
@@ -1705,7 +1695,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1" display="https://prettier.io/docs/en/rationale.html"/>
+    <hyperlink ref="F13" r:id="rId1" display="Prettier was used for code formatting. All code on the master branch of our repository was formatted by Prettier. Please follow this link if you’re interested in the kinds of decisions Prettier makes as a linter: https://prettier.io/docs/en/rationale.html&#10;All variables use camelCase and try to be quite descriptive in what they do, except in cases relating to libraries like Express where ‘req’/’res’/’err’ are the standard."/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>